<commit_message>
added particles showcase to GraphicsLevel
</commit_message>
<xml_diff>
--- a/GAM550 Game Engine Rubric.xlsx
+++ b/GAM550 Game Engine Rubric.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Aleksey\DigiPen\year5\Fall\Gam550\repo\cant_escape_games\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VS_2017_Projects\GAM550\cant_escape_games\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{051B402D-0B0B-4F87-A581-88D7D081CEA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E5C6DE0-6AD1-411E-AA05-3F005E421DBF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1018" uniqueCount="496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="495">
   <si>
     <t>GAME NAME</t>
   </si>
@@ -2583,10 +2583,16 @@
     <t>We have GPU based particle system that uses the geometry shader to manage the lifetime of the particles.</t>
   </si>
   <si>
-    <t>So far it renders any 3D models perfectly fine. Regarding the procedular 3D models, it only drwas box &amp; sphere for now, will add more.</t>
-  </si>
-  <si>
     <t>We are using Semi Implicit Euler method for calculating velocity and position each frame, and Gaus Seidel method when solving for constraints. We are also have Rigid  bodies.</t>
+  </si>
+  <si>
+    <t>we have torque computation</t>
+  </si>
+  <si>
+    <t>We do have gravity, and mass based collision responses. We also have friction.</t>
+  </si>
+  <si>
+    <t>We are using Dynamic Aabb tree to subdivide the space and consider collision only of the objects that are near to each other. We also using GJK and EPA algorithm  to detect collision of convex polygons. We a re usising constraints to simuilate Normal force and friction</t>
   </si>
   <si>
     <t>Input thread &amp; Resources Loading Thread &amp; Main Thread</t>
@@ -2597,15 +2603,6 @@
   <si>
     <t>Using csv files for each language
 Can be changed in runtime if required. Localized Strings are used from scripts directly.</t>
-  </si>
-  <si>
-    <t>Convex objects collision detection, static objects given infinite mass and not updated for gravity.</t>
-  </si>
-  <si>
-    <t>We do have gravity, airdrag, and mass based collision responses. We also have friction.</t>
-  </si>
-  <si>
-    <t>We are using Dynamic Aabb tree to subdivide the space and consider collision only of the objects that are near to each other, this is also used for raycasting (mouse select). We also using GJK and EPA algorithm  to detect collision of convex polygons. We a re usising constraints to simuilate Normal force and friction</t>
   </si>
 </sst>
 </file>
@@ -38626,8 +38623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7796A703-CB01-B546-96F6-2FF8CF6BC92E}">
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="I44" sqref="I44"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
@@ -38890,7 +38887,7 @@
       </c>
       <c r="C17" s="267"/>
       <c r="D17" s="70" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="E17" s="68" t="s">
         <v>453</v>
@@ -38909,7 +38906,7 @@
       </c>
       <c r="C18" s="267"/>
       <c r="D18" s="70" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="E18" s="68" t="s">
         <v>454</v>
@@ -39083,7 +39080,7 @@
       </c>
       <c r="C28" s="267"/>
       <c r="D28" s="70" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="E28" s="68" t="s">
         <v>453</v>
@@ -39116,11 +39113,9 @@
         <v>448</v>
       </c>
       <c r="C31" s="308"/>
-      <c r="D31" s="70" t="s">
-        <v>488</v>
-      </c>
+      <c r="D31" s="70"/>
       <c r="E31" s="68" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="F31" s="68" t="s">
         <v>100</v>
@@ -39139,7 +39134,7 @@
         <v>485</v>
       </c>
       <c r="E32" s="68" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
       <c r="F32" s="68" t="s">
         <v>100</v>
@@ -39275,7 +39270,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="77.25" thickBot="1">
+    <row r="41" spans="1:7" ht="43.15" customHeight="1" thickBot="1">
       <c r="A41" s="74" t="s">
         <v>405</v>
       </c>
@@ -39284,7 +39279,7 @@
       </c>
       <c r="C41" s="308"/>
       <c r="D41" s="70" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="E41" s="68" t="s">
         <v>454</v>
@@ -39294,7 +39289,7 @@
       </c>
       <c r="G41" s="70"/>
     </row>
-    <row r="42" spans="1:7" ht="51.75" thickBot="1">
+    <row r="42" spans="1:7" ht="43.15" customHeight="1" thickBot="1">
       <c r="A42" s="74" t="s">
         <v>406</v>
       </c>
@@ -39303,17 +39298,17 @@
       </c>
       <c r="C42" s="308"/>
       <c r="D42" s="70" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="E42" s="68" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="F42" s="68" t="s">
         <v>100</v>
       </c>
       <c r="G42" s="70"/>
     </row>
-    <row r="43" spans="1:7" ht="39" thickBot="1">
+    <row r="43" spans="1:7" ht="43.15" customHeight="1" thickBot="1">
       <c r="A43" s="74" t="s">
         <v>407</v>
       </c>
@@ -39322,7 +39317,7 @@
       </c>
       <c r="C43" s="308"/>
       <c r="D43" s="70" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="E43" s="68" t="s">
         <v>454</v>
@@ -39332,7 +39327,7 @@
       </c>
       <c r="G43" s="70"/>
     </row>
-    <row r="44" spans="1:7" ht="141" thickBot="1">
+    <row r="44" spans="1:7" ht="43.15" customHeight="1" thickBot="1">
       <c r="A44" s="74" t="s">
         <v>408</v>
       </c>
@@ -39341,7 +39336,7 @@
       </c>
       <c r="C44" s="308"/>
       <c r="D44" s="70" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="E44" s="68" t="s">
         <v>454</v>
@@ -44596,16 +44591,8 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31F51AB6-4F4A-4993-A4C1-F432D850217F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="1528dd05-61d3-4f6f-8f4b-07c6ec116598"/>
-    <ds:schemaRef ds:uri="de65e86b-0f7f-4b92-a9bd-18bee373006c"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>